<commit_message>
Have MUMPS converter figure out for itself whether days or seconds are used.
</commit_message>
<xml_diff>
--- a/DECS Excel Add-Ins/test files/MUMPS dates.xlsx
+++ b/DECS Excel Add-Ins/test files/MUMPS dates.xlsx
@@ -8,36 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\DECS-Office-AddIns\DECS Excel Add-Ins\test files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69F6836-8C7E-4BA4-8B5A-FCFD2FBB1E62}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362D3A66-6638-4C2B-8C81-55276DA2E88A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{21A029B3-2C69-481C-BB7E-3DD9DD8D06BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{21A029B3-2C69-481C-BB7E-3DD9DD8D06BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Answer" sheetId="2" r:id="rId1"/>
-    <sheet name="Test" sheetId="3" r:id="rId2"/>
+    <sheet name="Seconds" sheetId="3" r:id="rId2"/>
+    <sheet name="Days" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>MUMPS Conversion</t>
   </si>
@@ -104,7 +94,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -113,6 +103,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1114,7 +1106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0AF2061-FDA0-448C-93F7-720097CEEC23}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1177,4 +1169,82 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C717FD05-633F-4B04-8FD2-D8A6F75BE983}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" style="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <f>Answer!A2/86400</f>
+        <v>64557.37228009259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <f>Answer!A3/86400</f>
+        <v>64558.355787037035</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <f>Answer!A4/86400</f>
+        <v>64558.355787037035</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <f>Answer!A5/86400</f>
+        <v>64575.556620370371</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <f>Answer!A6/86400</f>
+        <v>64558.353356481479</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <f>Answer!A7/86400</f>
+        <v>64557.436967592592</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <f>Answer!A8/86400</f>
+        <v>64557.436967592592</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <f>Answer!A9/86400</f>
+        <v>64557.436967592592</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <f>Answer!A10/86400</f>
+        <v>64557.436979166669</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>